<commit_message>
Updates to Initalisation form
Fixed bug in saving initialisation file from GUI for a stage-structured
population and revised format of GUI initialisation file to be similar
to batch initialisation file
</commit_message>
<xml_diff>
--- a/doc/RS_v2.0_distribution.xlsx
+++ b/doc/RS_v2.0_distribution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter_v2_0\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <author>Steve Palmer</author>
   </authors>
   <commentList>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -823,110 +823,113 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3">
-        <v>170419</v>
+        <v>170430</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3">
         <v>170430</v>
       </c>
-      <c r="D12" t="s">
-        <v>29</v>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3">
         <v>170430</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>45</v>
+      <c r="D13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
+      <c r="A14" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="3">
         <v>170430</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="3">
-        <v>170430</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5">
+        <v>171027</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>37</v>
+      <c r="A16" t="s">
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
-        <v>171027</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>38</v>
+      <c r="C16" s="3">
+        <v>171205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
+      <c r="A17" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="3">
-        <v>171205</v>
+        <v>47</v>
+      </c>
+      <c r="C17" s="5">
+        <v>180103</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C18" s="5">
-        <v>180103</v>
+        <v>180112</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -934,16 +937,13 @@
       <c r="C19" s="5">
         <v>180112</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>49</v>
+      <c r="A20" t="s">
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5">
         <v>180112</v>
@@ -951,21 +951,21 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5">
-        <v>180112</v>
+        <v>180417</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C22" s="5">
         <v>180417</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -984,10 +984,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C24" s="5">
         <v>180417</v>
@@ -995,13 +995,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="5">
-        <v>180417</v>
+        <v>16</v>
+      </c>
+      <c r="C25" s="3">
+        <v>180822</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1113,6 +1113,9 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>180822</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>